<commit_message>
updates to grades. added extra credit assignment
</commit_message>
<xml_diff>
--- a/Grades.xlsx
+++ b/Grades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncc\Fall-2018---CIS7---Discrete-Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Anzo, Alan F.</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Ramirez, Brandon A</t>
+  </si>
+  <si>
+    <t>Please See Me</t>
+  </si>
+  <si>
+    <t>********</t>
   </si>
 </sst>
 </file>
@@ -193,7 +199,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +215,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCBCBA8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -241,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -253,6 +265,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,9 +596,10 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>30</v>
       </c>
@@ -624,30 +642,48 @@
       <c r="P1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>20</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
-      </c>
-      <c r="O2">
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6">
         <f>SUM(B2:N2)</f>
-        <v>60</v>
-      </c>
-      <c r="P2" s="4">
+        <v>120</v>
+      </c>
+      <c r="P2" s="7">
         <f>O2/$O$34</f>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -658,27 +694,33 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
       <c r="G3">
         <v>20</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O34" si="0">SUM(B3:N3)</f>
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="P3" s="4">
-        <f t="shared" ref="O3:P34" si="1">O3/$O$34</f>
-        <v>0.8214285714285714</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="P3:P34" si="1">O3/$O$34</f>
+        <v>0.9642857142857143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -688,6 +730,9 @@
       <c r="C4">
         <v>20</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="O4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -697,7 +742,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -710,6 +755,9 @@
       <c r="D5">
         <v>20</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>20</v>
       </c>
@@ -728,7 +776,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -741,6 +789,9 @@
       <c r="D6">
         <v>20</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <v>20</v>
       </c>
@@ -762,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -775,6 +826,9 @@
       <c r="D7">
         <v>20</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <v>20</v>
       </c>
@@ -793,7 +847,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -806,6 +860,9 @@
       <c r="D8">
         <v>20</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
       <c r="F8">
         <v>16</v>
       </c>
@@ -821,7 +878,7 @@
         <v>0.54285714285714282</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -834,25 +891,31 @@
       <c r="D9">
         <v>25</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
         <v>20</v>
       </c>
       <c r="G9">
         <v>20</v>
       </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
       <c r="I9">
         <v>20</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" si="1"/>
-        <v>0.8928571428571429</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.0357142857142858</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -862,6 +925,9 @@
       <c r="D10">
         <v>20</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
       <c r="G10">
         <v>20</v>
       </c>
@@ -874,7 +940,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -887,6 +953,9 @@
       <c r="D11">
         <v>25</v>
       </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
       <c r="F11">
         <v>20</v>
       </c>
@@ -908,10 +977,13 @@
         <v>1.0357142857142858</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
       <c r="I12">
         <v>20</v>
       </c>
@@ -924,29 +996,35 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13">
         <v>25</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="F13">
         <v>20</v>
       </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
       <c r="H13">
         <v>20</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" si="1"/>
-        <v>0.4642857142857143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.6071428571428571</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -959,6 +1037,9 @@
       <c r="D14">
         <v>25</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
       <c r="F14">
         <v>20</v>
       </c>
@@ -980,7 +1061,7 @@
         <v>1.0357142857142858</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -990,6 +1071,12 @@
       <c r="C15">
         <v>15</v>
       </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15">
         <v>20</v>
       </c>
@@ -1001,20 +1088,23 @@
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>0.6785714285714286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.8214285714285714</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16">
         <v>20</v>
       </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
       <c r="O16">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1024,23 +1114,47 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:17" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="6">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6">
+        <v>20</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>20</v>
+      </c>
+      <c r="G17" s="6">
+        <v>20</v>
+      </c>
+      <c r="H17" s="6">
+        <v>20</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" si="1"/>
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="O18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1050,10 +1164,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
       <c r="O19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1063,10 +1180,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
       <c r="O20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1076,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1089,28 +1209,37 @@
       <c r="D21">
         <v>25</v>
       </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="F21">
         <v>20</v>
       </c>
       <c r="G21">
         <v>20</v>
       </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
       <c r="I21">
         <v>20</v>
       </c>
       <c r="O21">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
       <c r="O22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1120,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1130,6 +1259,9 @@
       <c r="C23">
         <v>20</v>
       </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
       <c r="O23">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1139,32 +1271,41 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D24">
         <v>20</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
       <c r="F24">
         <v>18</v>
       </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+      <c r="H24">
+        <v>20</v>
+      </c>
       <c r="O24">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="1"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.84285714285714286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1174,16 +1315,34 @@
       <c r="C25">
         <v>20</v>
       </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
+      </c>
+      <c r="H25">
+        <v>20</v>
+      </c>
+      <c r="I25">
+        <v>20</v>
+      </c>
       <c r="O25">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="1"/>
-        <v>0.2857142857142857</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1196,6 +1355,9 @@
       <c r="D26">
         <v>20</v>
       </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
       <c r="O26">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1205,7 +1367,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1218,6 +1380,9 @@
       <c r="D27">
         <v>25</v>
       </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
       <c r="O27">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1227,10 +1392,13 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
       <c r="O28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1240,10 +1408,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
       <c r="O29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1253,41 +1424,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+      <c r="G30">
+        <v>20</v>
+      </c>
+      <c r="H30">
+        <v>20</v>
+      </c>
+      <c r="I30">
+        <v>20</v>
+      </c>
       <c r="O30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.9642857142857143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>20</v>
       </c>
       <c r="O31">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="P31" s="4">
         <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.48571428571428571</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C32">
         <v>10</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
       </c>
       <c r="O32">
         <f t="shared" si="0"/>
@@ -1310,6 +1520,9 @@
       </c>
       <c r="D33">
         <v>20</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
       </c>
       <c r="G33">
         <v>20</v>

</xml_diff>